<commit_message>
Revise calculation of req'd batteries
If specified 6V batteries, require an even number. If 12V batteries,
round calculated number up (ceiling) instead of nearest integer.
</commit_message>
<xml_diff>
--- a/engr/power.xlsx
+++ b/engr/power.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="563"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="563" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Consumption" sheetId="1" r:id="rId1"/>
@@ -46,6 +46,40 @@
           </rPr>
           <t xml:space="preserve">
 Assuming vertical wind speed is normally distributed and deadband multiplier is 0.85</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Patrick O'Keeffe</author>
+  </authors>
+  <commentList>
+    <comment ref="F14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Choices: 6, 12</t>
         </r>
       </text>
     </comment>
@@ -1054,7 +1088,7 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1522,14 +1556,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1857,8 +1891,8 @@
         <v>85</v>
       </c>
       <c r="F18" s="27">
-        <f>(B17/F15)*(B13/F14)</f>
-        <v>5.3421087022900782</v>
+        <f>IF(F14&lt;12, EVEN((B17/F15)*(B13/F14)), CEILING((B17/F15)*(B13/F14),1))</f>
+        <v>6</v>
       </c>
       <c r="G18" t="s">
         <v>81</v>
@@ -2096,5 +2130,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>